<commit_message>
Added GME and AMC to companies list
</commit_message>
<xml_diff>
--- a/Companies.xlsx
+++ b/Companies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\DSE203_FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DA1C22-819F-4350-8E28-EF8983156A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE527319-A4C5-48D0-9B28-7D03721BFCCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{36B6ED52-09F6-46EE-9859-B5446CFE7247}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="233">
   <si>
     <t>Symbol</t>
   </si>
@@ -718,6 +718,24 @@
   </si>
   <si>
     <t>zebra</t>
+  </si>
+  <si>
+    <t>GME</t>
+  </si>
+  <si>
+    <t>AMC</t>
+  </si>
+  <si>
+    <t>AMC Entertainment Holdings Inc</t>
+  </si>
+  <si>
+    <t>amc entertainment holdings, amc entertainment</t>
+  </si>
+  <si>
+    <t>GameStop Corp</t>
+  </si>
+  <si>
+    <t>gamestop, gamestop corporation</t>
   </si>
 </sst>
 </file>
@@ -1072,10 +1090,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B1CDED0-334C-4396-9929-7EF6E85E09DA}">
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1921,6 +1939,28 @@
         <v>226</v>
       </c>
     </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C77" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C78" t="s">
+        <v>230</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B76" xr:uid="{6B1CDED0-334C-4396-9929-7EF6E85E09DA}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>